<commit_message>
Created project outputs for all v2 boards
</commit_message>
<xml_diff>
--- a/systems/sys_debug_pcb/Project Outputs for syspcb/syspcb.xlsx
+++ b/systems/sys_debug_pcb/Project Outputs for syspcb/syspcb.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{067DAEEC-31A9-4CB6-B703-FD72A79CE63D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan Vogel\Files\Coding Projects\pcbs\systems\sys_debug_pcb\Project Outputs for syspcb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C90999-DDEA-4369-B9FB-A74B69B74D55}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="8490" xr2:uid="{754DE07C-88B6-4A90-B7A9-C6D831812ABB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14378" windowHeight="8490" xr2:uid="{754DE07C-88B6-4A90-B7A9-C6D831812ABB}"/>
   </bookViews>
   <sheets>
     <sheet name="syspcb" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="76">
   <si>
     <t>Line #</t>
   </si>
@@ -139,9 +144,6 @@
     <t>EPS1</t>
   </si>
   <si>
-    <t>Header, 2-Pin</t>
-  </si>
-  <si>
     <t>P3</t>
   </si>
   <si>
@@ -157,9 +159,6 @@
     <t>P7</t>
   </si>
   <si>
-    <t>HDR2X3</t>
-  </si>
-  <si>
     <t>Header, 3-Pin, Dual row</t>
   </si>
   <si>
@@ -169,18 +168,12 @@
     <t>Header 4X2A</t>
   </si>
   <si>
-    <t>Header, 4-Pin, Dual row</t>
-  </si>
-  <si>
     <t>CANH</t>
   </si>
   <si>
     <t>Header 10X2A</t>
   </si>
   <si>
-    <t>Header, 10-Pin, Dual row</t>
-  </si>
-  <si>
     <t>P1, P2</t>
   </si>
   <si>
@@ -202,9 +195,6 @@
     <t>182-25ME-ND</t>
   </si>
   <si>
-    <t>Res2</t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -242,6 +232,33 @@
   </si>
   <si>
     <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15, D16, D17, D19, D20</t>
+  </si>
+  <si>
+    <t>Header, 2-Pin, Female</t>
+  </si>
+  <si>
+    <t>Programming Header</t>
+  </si>
+  <si>
+    <t>Header, 4-Pin, Dual row, Female</t>
+  </si>
+  <si>
+    <t>Header, 10-Pin, Dual row, Female</t>
+  </si>
+  <si>
+    <t>SAM1085-02-ND</t>
+  </si>
+  <si>
+    <t>SAM10846-ND</t>
+  </si>
+  <si>
+    <t>SAM1084-04-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAM10958-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-330HRCT-ND </t>
   </si>
 </sst>
 </file>
@@ -271,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,6 +298,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,6 +344,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -638,24 +669,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D001B7-D462-41E7-A66F-478F05233605}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="9.90625" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" customWidth="1"/>
-    <col min="7" max="7" width="25.6328125" customWidth="1"/>
-    <col min="8" max="8" width="22.453125" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" customWidth="1"/>
-    <col min="10" max="10" width="21.90625" customWidth="1"/>
-    <col min="11" max="11" width="19.6328125" customWidth="1"/>
-    <col min="12" max="12" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="9.9296875" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
+    <col min="3" max="3" width="39.3984375" customWidth="1"/>
+    <col min="4" max="4" width="13.265625" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" customWidth="1"/>
+    <col min="6" max="6" width="16.265625" customWidth="1"/>
+    <col min="7" max="7" width="25.59765625" customWidth="1"/>
+    <col min="8" max="8" width="22.46484375" customWidth="1"/>
+    <col min="9" max="9" width="12.46484375" customWidth="1"/>
+    <col min="10" max="10" width="21.9296875" customWidth="1"/>
+    <col min="11" max="11" width="19.59765625" customWidth="1"/>
+    <col min="12" max="12" width="18.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -731,7 +765,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -769,7 +803,7 @@
         <v>0.75707000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -807,7 +841,7 @@
         <v>6.59</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -845,7 +879,7 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -853,10 +887,10 @@
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -873,24 +907,24 @@
       <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>12</v>
+      <c r="J6" t="s">
+        <v>71</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -907,24 +941,24 @@
       <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>12</v>
+      <c r="J7" t="s">
+        <v>71</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -941,24 +975,24 @@
       <c r="I8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>12</v>
+      <c r="J8" t="s">
+        <v>71</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="E9" s="3">
         <v>3</v>
@@ -975,24 +1009,24 @@
       <c r="I9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>12</v>
+      <c r="J9" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -1009,24 +1043,24 @@
       <c r="I10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>12</v>
+      <c r="J10" t="s">
+        <v>73</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E11" s="3">
         <v>2</v>
@@ -1043,33 +1077,33 @@
       <c r="I11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>12</v>
+      <c r="J11" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>17</v>
@@ -1078,7 +1112,7 @@
         <v>18</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K12" s="3">
         <v>3.44</v>
@@ -1087,18 +1121,18 @@
         <v>3.44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>58</v>
+      <c r="B13" s="5">
+        <v>330</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3">
         <v>19</v>
@@ -1115,117 +1149,117 @@
       <c r="I13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>12</v>
+      <c r="J13" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="7">
+        <v>2</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" s="7">
+        <v>0.91646000000000005</v>
+      </c>
+      <c r="L14" s="7">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="3">
-        <v>2</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="E15" s="7">
+        <v>3</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="K14" s="3">
-        <v>0.91646000000000005</v>
-      </c>
-      <c r="L14" s="3">
-        <v>1.83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="D16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="3">
-        <v>3</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="E16" s="7">
         <v>19</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="F16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1243,28 +1277,21 @@
     <hyperlink ref="J5" r:id="rId12" tooltip="Supplier" display="'401-2000-ND" xr:uid="{37F0BC2A-C4BF-4FBA-AD4C-5673F17F7178}"/>
     <hyperlink ref="F6" tooltip="Component" display="'" xr:uid="{85DA65C2-A123-4461-BA42-7E34A59D7201}"/>
     <hyperlink ref="G6" tooltip="Manufacturer" display="'" xr:uid="{97722D9B-B80F-4F0D-A8FF-38448776451D}"/>
-    <hyperlink ref="J6" tooltip="Supplier" display="'" xr:uid="{7EAFDE14-DD0B-4BD6-8013-88AEC192E7D0}"/>
     <hyperlink ref="F7" tooltip="Component" display="'" xr:uid="{30ACD6D5-62C9-4CAE-98CA-C92DA22C911C}"/>
     <hyperlink ref="G7" tooltip="Manufacturer" display="'" xr:uid="{75F02657-E86B-4738-AAD6-9A3A729CB499}"/>
-    <hyperlink ref="J7" tooltip="Supplier" display="'" xr:uid="{77FE9D38-C6D6-4168-BAEA-1E28511F851E}"/>
     <hyperlink ref="F8" tooltip="Component" display="'" xr:uid="{EDA9B5EC-4136-4437-BD75-AAB2AE141640}"/>
     <hyperlink ref="G8" tooltip="Manufacturer" display="'" xr:uid="{9D830982-7E02-497C-9A8E-F1B2CBA7008F}"/>
-    <hyperlink ref="J8" tooltip="Supplier" display="'" xr:uid="{A6C49741-8871-4321-B53A-576675E4ECEC}"/>
     <hyperlink ref="F9" tooltip="Component" display="'" xr:uid="{AC4A38E6-772F-43C0-8E07-BC6783975FE0}"/>
     <hyperlink ref="G9" tooltip="Manufacturer" display="'" xr:uid="{31E01EEF-F103-470F-BBE2-D90689F5EF92}"/>
-    <hyperlink ref="J9" tooltip="Supplier" display="'" xr:uid="{D80033AF-79D8-4EDD-89F3-E91AF975B4E5}"/>
     <hyperlink ref="F10" tooltip="Component" display="'" xr:uid="{5DEB86BB-FA19-4E78-BF24-C526FECA068C}"/>
     <hyperlink ref="G10" tooltip="Manufacturer" display="'" xr:uid="{6D2F0A0E-7048-4E42-9D5B-377D1AE79772}"/>
-    <hyperlink ref="J10" tooltip="Supplier" display="'" xr:uid="{3ADE116F-1E3E-431E-8AD6-F9CCF73C1D4A}"/>
     <hyperlink ref="F11" tooltip="Component" display="'" xr:uid="{631B84FC-799D-4AE4-B2B9-87D068AC7ED4}"/>
     <hyperlink ref="G11" tooltip="Manufacturer" display="'" xr:uid="{E4FD1A67-49D5-4C03-8BB4-890341797DC9}"/>
-    <hyperlink ref="J11" tooltip="Supplier" display="'" xr:uid="{B7BD67C1-4CEC-4DC4-A98A-96559260873C}"/>
     <hyperlink ref="F12" r:id="rId13" tooltip="Component" display="'NorComp" xr:uid="{7BD57982-2757-463F-A321-4FD729972188}"/>
     <hyperlink ref="G12" r:id="rId14" tooltip="Manufacturer" display="'182-025-113R531" xr:uid="{0FD47AE4-6648-4F7C-AAAE-F571EBDA3360}"/>
     <hyperlink ref="J12" r:id="rId15" tooltip="Supplier" display="'182-25ME-ND" xr:uid="{2FB3BE83-B869-44FF-A256-52E9058D96D6}"/>
     <hyperlink ref="F13" tooltip="Component" display="'" xr:uid="{9ACF65B6-2ABD-4857-9A38-3A462A1DCF61}"/>
     <hyperlink ref="G13" tooltip="Manufacturer" display="'" xr:uid="{A7E26BFD-23F8-409E-A814-4DA9C9C6D5C1}"/>
-    <hyperlink ref="J13" tooltip="Supplier" display="'" xr:uid="{05B8C699-3020-4BB9-98EB-5976483BEE2E}"/>
     <hyperlink ref="F14" r:id="rId16" tooltip="Component" display="'Wurth Electronics" xr:uid="{CABC8161-1634-483F-B930-7FA25B2B482E}"/>
     <hyperlink ref="G14" r:id="rId17" tooltip="Manufacturer" display="'691102710002" xr:uid="{236BA851-4984-4BBF-8521-49D841E1E8E3}"/>
     <hyperlink ref="J14" r:id="rId18" tooltip="Supplier" display="'732-2028-ND" xr:uid="{66B1F2D1-F21D-461C-8AE1-60EBEA295430}"/>
@@ -1274,8 +1301,11 @@
     <hyperlink ref="F16" tooltip="Component" display="'" xr:uid="{AF932B54-9B26-411D-B72C-56AD9116CEA7}"/>
     <hyperlink ref="G16" tooltip="Manufacturer" display="'" xr:uid="{5F806116-3EB7-427F-A5B7-9BE24922C07E}"/>
     <hyperlink ref="J16" tooltip="Supplier" display="'" xr:uid="{EDDA0C2B-D047-41DD-BC25-116F02829D3D}"/>
+    <hyperlink ref="J9" r:id="rId19" display="https://www.digikey.ca/product-detail/en/samtec-inc/TSW-103-07-F-D/SAM10846-ND/2685876" xr:uid="{01B4601F-4B2B-4FA1-BFB5-33C54CDBBE72}"/>
+    <hyperlink ref="J11" r:id="rId20" display="https://www.digikey.ca/product-detail/en/samtec-inc/CES-110-01-L-D/SAM10958-ND/6693052" xr:uid="{34870044-205A-4007-8D92-C235F8529D9E}"/>
+    <hyperlink ref="J13" r:id="rId21" display="https://www.digikey.ca/product-detail/en/yageo/RC0603FR-07330RL/311-330HRCT-ND/730109" xr:uid="{3699C34F-7B51-44F8-9880-ACA92B39DC65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId19"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>